<commit_message>
Initial import of Telegram birthday autoresponder
</commit_message>
<xml_diff>
--- a/birthdays.xlsx
+++ b/birthdays.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>phone</t>
   </si>
@@ -25,16 +25,7 @@
     <t>other_name</t>
   </si>
   <si>
-    <t>Garv</t>
-  </si>
-  <si>
-    <t>Anoop</t>
-  </si>
-  <si>
-    <t>sdfsd</t>
-  </si>
-  <si>
-    <t>fsdf</t>
+    <t>Shalin</t>
   </si>
 </sst>
 </file>
@@ -322,7 +313,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>9.18057148934E11</v>
+        <v>9.19967488889E11</v>
       </c>
       <c r="B2" s="3">
         <v>45841.0</v>
@@ -331,22 +322,11 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
-        <v>9.18807420329E11</v>
-      </c>
-      <c r="B3" s="3">
-        <v>45841.0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>